<commit_message>
- Changed contact person from Priska to Mike Hoopmann. - Updated sample submission form.
</commit_message>
<xml_diff>
--- a/WebRoot/costcenter_resources/UWPR sample submission form.xlsx
+++ b/WebRoot/costcenter_resources/UWPR sample submission form.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PriskaStuff\UWPR costcenter\SampleSubmissionForm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31ACF114-C205-4E85-B7C9-98A5BBBC1E6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4CB54E-C9F7-410F-92EB-6C625ECD2E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -408,9 +408,6 @@
     </r>
   </si>
   <si>
-    <t>Then complete this form and upload it to your project online and email priska@uw.edu to coordinate a time to drop off your samples.</t>
-  </si>
-  <si>
     <t>Principal Investigator (PI):</t>
   </si>
   <si>
@@ -1639,6 +1636,9 @@
   </si>
   <si>
     <t>Revised 9/1/25</t>
+  </si>
+  <si>
+    <t>Then complete this form and upload it to your project online and email hoopmann@uw.edu to coordinate a time to drop off your samples.</t>
   </si>
 </sst>
 </file>
@@ -3423,9 +3423,75 @@
     <xf numFmtId="0" fontId="76" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="8" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3434,72 +3500,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="10" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3825,8 +3825,8 @@
             <a:xfrm>
               <a:off x="3924300" y="10115550"/>
               <a:ext cx="1371600" cy="209550"/>
-              <a:chOff x="2266950" y="4686300"/>
-              <a:chExt cx="1685925" cy="209550"/>
+              <a:chOff x="2266949" y="4686300"/>
+              <a:chExt cx="1685926" cy="209550"/>
             </a:xfrm>
           </xdr:grpSpPr>
           <xdr:sp macro="" textlink="">
@@ -3845,7 +3845,7 @@
             </xdr:nvSpPr>
             <xdr:spPr bwMode="auto">
               <a:xfrm>
-                <a:off x="2266950" y="4686300"/>
+                <a:off x="2266949" y="4686300"/>
                 <a:ext cx="781050" cy="209550"/>
               </a:xfrm>
               <a:prstGeom prst="rect">
@@ -5539,8 +5539,8 @@
             <a:xfrm>
               <a:off x="2943225" y="3743325"/>
               <a:ext cx="1466850" cy="209550"/>
-              <a:chOff x="2266950" y="4686300"/>
-              <a:chExt cx="1685925" cy="209550"/>
+              <a:chOff x="2266949" y="4686300"/>
+              <a:chExt cx="1685926" cy="209550"/>
             </a:xfrm>
           </xdr:grpSpPr>
           <xdr:sp macro="" textlink="">
@@ -5559,7 +5559,7 @@
             </xdr:nvSpPr>
             <xdr:spPr bwMode="auto">
               <a:xfrm>
-                <a:off x="2266950" y="4686300"/>
+                <a:off x="2266949" y="4686300"/>
                 <a:ext cx="781050" cy="209550"/>
               </a:xfrm>
               <a:prstGeom prst="rect">
@@ -15118,7 +15118,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP128"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15257,7 +15259,7 @@
     </row>
     <row r="7" spans="1:42" s="156" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="153" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C7" s="153"/>
       <c r="D7" s="153"/>
@@ -15285,7 +15287,7 @@
     </row>
     <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="C8" s="97" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D8" s="65"/>
       <c r="P8" s="94"/>
@@ -15308,7 +15310,7 @@
     </row>
     <row r="10" spans="1:42" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="68" t="s">
-        <v>42</v>
+        <v>298</v>
       </c>
       <c r="C10" s="97"/>
       <c r="D10" s="97"/>
@@ -15322,7 +15324,7 @@
     </row>
     <row r="11" spans="1:42" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="99" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C11" s="97"/>
       <c r="D11" s="97"/>
@@ -15353,7 +15355,7 @@
     <row r="13" spans="1:42" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="170"/>
       <c r="B13" s="244" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C13" s="245"/>
       <c r="D13" s="245"/>
@@ -15378,16 +15380,16 @@
     <row r="14" spans="1:42" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="170"/>
       <c r="B14" s="248" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="306"/>
-      <c r="D14" s="306"/>
+        <v>42</v>
+      </c>
+      <c r="C14" s="304"/>
+      <c r="D14" s="304"/>
       <c r="E14" s="170"/>
       <c r="F14" s="248" t="s">
-        <v>273</v>
-      </c>
-      <c r="G14" s="300"/>
-      <c r="H14" s="300"/>
+        <v>272</v>
+      </c>
+      <c r="G14" s="297"/>
+      <c r="H14" s="297"/>
       <c r="I14" s="272"/>
       <c r="P14" s="94"/>
       <c r="Q14" s="94"/>
@@ -15400,16 +15402,16 @@
     <row r="15" spans="1:42" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="170"/>
       <c r="B15" s="269" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" s="242"/>
       <c r="D15" s="241"/>
       <c r="E15" s="170"/>
       <c r="F15" s="248" t="s">
-        <v>264</v>
-      </c>
-      <c r="G15" s="307"/>
-      <c r="H15" s="308"/>
+        <v>263</v>
+      </c>
+      <c r="G15" s="305"/>
+      <c r="H15" s="306"/>
       <c r="I15" s="272"/>
       <c r="P15" s="94"/>
       <c r="Q15" s="94"/>
@@ -15422,18 +15424,18 @@
     <row r="16" spans="1:42" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="170"/>
       <c r="B16" s="248" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="309"/>
-      <c r="D16" s="309"/>
+        <v>45</v>
+      </c>
+      <c r="C16" s="307"/>
+      <c r="D16" s="307"/>
       <c r="E16" s="170"/>
       <c r="F16" s="250" t="s">
-        <v>265</v>
-      </c>
-      <c r="G16" s="315" t="s">
-        <v>270</v>
-      </c>
-      <c r="H16" s="316"/>
+        <v>264</v>
+      </c>
+      <c r="G16" s="294" t="s">
+        <v>269</v>
+      </c>
+      <c r="H16" s="295"/>
       <c r="I16" s="272"/>
       <c r="K16" s="98"/>
       <c r="L16" s="98"/>
@@ -15456,18 +15458,18 @@
     <row r="17" spans="1:41" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="170"/>
       <c r="B17" s="250" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="310"/>
-      <c r="D17" s="310"/>
+        <v>46</v>
+      </c>
+      <c r="C17" s="308"/>
+      <c r="D17" s="308"/>
       <c r="E17" s="170"/>
       <c r="F17" s="250" t="s">
-        <v>266</v>
-      </c>
-      <c r="G17" s="315" t="s">
-        <v>271</v>
-      </c>
-      <c r="H17" s="316"/>
+        <v>265</v>
+      </c>
+      <c r="G17" s="294" t="s">
+        <v>270</v>
+      </c>
+      <c r="H17" s="295"/>
       <c r="I17" s="272"/>
       <c r="J17" s="86"/>
       <c r="K17" s="98"/>
@@ -15491,18 +15493,18 @@
     <row r="18" spans="1:41" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="170"/>
       <c r="B18" s="273" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="311"/>
-      <c r="D18" s="311"/>
+        <v>43</v>
+      </c>
+      <c r="C18" s="309"/>
+      <c r="D18" s="309"/>
       <c r="E18" s="270"/>
       <c r="F18" s="251" t="s">
-        <v>267</v>
-      </c>
-      <c r="G18" s="317" t="s">
-        <v>272</v>
-      </c>
-      <c r="H18" s="317"/>
+        <v>266</v>
+      </c>
+      <c r="G18" s="296" t="s">
+        <v>271</v>
+      </c>
+      <c r="H18" s="296"/>
       <c r="I18" s="274"/>
       <c r="J18" s="86"/>
       <c r="K18" s="98"/>
@@ -15548,7 +15550,7 @@
     </row>
     <row r="20" spans="1:41" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="244" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C20" s="233"/>
       <c r="D20" s="233"/>
@@ -15574,15 +15576,15 @@
     <row r="21" spans="1:41" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="170"/>
       <c r="B21" s="248" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="301"/>
-      <c r="D21" s="301"/>
-      <c r="E21" s="301"/>
-      <c r="F21" s="301"/>
-      <c r="G21" s="301"/>
-      <c r="H21" s="301"/>
-      <c r="I21" s="302"/>
+        <v>47</v>
+      </c>
+      <c r="C21" s="298"/>
+      <c r="D21" s="298"/>
+      <c r="E21" s="298"/>
+      <c r="F21" s="298"/>
+      <c r="G21" s="298"/>
+      <c r="H21" s="298"/>
+      <c r="I21" s="299"/>
       <c r="P21" s="94"/>
       <c r="Q21" s="94"/>
       <c r="R21" s="94"/>
@@ -15600,15 +15602,15 @@
     <row r="22" spans="1:41" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="170"/>
       <c r="B22" s="248" t="s">
-        <v>255</v>
-      </c>
-      <c r="C22" s="301"/>
-      <c r="D22" s="301"/>
-      <c r="E22" s="301"/>
-      <c r="F22" s="301"/>
-      <c r="G22" s="301"/>
-      <c r="H22" s="301"/>
-      <c r="I22" s="302"/>
+        <v>254</v>
+      </c>
+      <c r="C22" s="298"/>
+      <c r="D22" s="298"/>
+      <c r="E22" s="298"/>
+      <c r="F22" s="298"/>
+      <c r="G22" s="298"/>
+      <c r="H22" s="298"/>
+      <c r="I22" s="299"/>
       <c r="J22" s="98"/>
       <c r="N22" s="171"/>
       <c r="O22" s="171"/>
@@ -15635,15 +15637,15 @@
     <row r="23" spans="1:41" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="170"/>
       <c r="B23" s="248" t="s">
-        <v>282</v>
-      </c>
-      <c r="C23" s="301"/>
-      <c r="D23" s="301"/>
-      <c r="E23" s="301"/>
-      <c r="F23" s="301"/>
-      <c r="G23" s="301"/>
-      <c r="H23" s="301"/>
-      <c r="I23" s="302"/>
+        <v>281</v>
+      </c>
+      <c r="C23" s="298"/>
+      <c r="D23" s="298"/>
+      <c r="E23" s="298"/>
+      <c r="F23" s="298"/>
+      <c r="G23" s="298"/>
+      <c r="H23" s="298"/>
+      <c r="I23" s="299"/>
       <c r="J23" s="98"/>
       <c r="N23" s="171"/>
       <c r="O23" s="171"/>
@@ -15669,16 +15671,16 @@
     </row>
     <row r="24" spans="1:41" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="170"/>
-      <c r="B24" s="303" t="s">
-        <v>240</v>
-      </c>
-      <c r="C24" s="304"/>
-      <c r="D24" s="304"/>
-      <c r="E24" s="304"/>
-      <c r="F24" s="304"/>
-      <c r="G24" s="304"/>
-      <c r="H24" s="304"/>
-      <c r="I24" s="305"/>
+      <c r="B24" s="300" t="s">
+        <v>239</v>
+      </c>
+      <c r="C24" s="301"/>
+      <c r="D24" s="301"/>
+      <c r="E24" s="301"/>
+      <c r="F24" s="301"/>
+      <c r="G24" s="301"/>
+      <c r="H24" s="301"/>
+      <c r="I24" s="302"/>
       <c r="P24" s="94"/>
       <c r="Q24" s="94"/>
       <c r="R24" s="94"/>
@@ -15694,14 +15696,14 @@
       <c r="AO24" s="81"/>
     </row>
     <row r="25" spans="1:41" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="303"/>
-      <c r="C25" s="304"/>
-      <c r="D25" s="304"/>
-      <c r="E25" s="304"/>
-      <c r="F25" s="304"/>
-      <c r="G25" s="304"/>
-      <c r="H25" s="304"/>
-      <c r="I25" s="305"/>
+      <c r="B25" s="300"/>
+      <c r="C25" s="301"/>
+      <c r="D25" s="301"/>
+      <c r="E25" s="301"/>
+      <c r="F25" s="301"/>
+      <c r="G25" s="301"/>
+      <c r="H25" s="301"/>
+      <c r="I25" s="302"/>
       <c r="P25" s="94"/>
       <c r="Q25" s="94"/>
       <c r="R25" s="94"/>
@@ -15718,17 +15720,17 @@
     </row>
     <row r="26" spans="1:41" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="279" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C26" s="278">
         <v>1</v>
       </c>
-      <c r="D26" s="313">
+      <c r="D26" s="292">
         <f>ROUNDUP((2+($C26*$C27*140)/60),0)</f>
         <v>5</v>
       </c>
-      <c r="E26" s="314" t="s">
-        <v>294</v>
+      <c r="E26" s="293" t="s">
+        <v>293</v>
       </c>
       <c r="F26" s="235"/>
       <c r="G26" s="235"/>
@@ -15750,13 +15752,13 @@
     </row>
     <row r="27" spans="1:41" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="281" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C27" s="243">
         <v>1</v>
       </c>
-      <c r="D27" s="313"/>
-      <c r="E27" s="314"/>
+      <c r="D27" s="292"/>
+      <c r="E27" s="293"/>
       <c r="F27" s="235"/>
       <c r="G27" s="235"/>
       <c r="H27" s="235"/>
@@ -15777,7 +15779,7 @@
     </row>
     <row r="28" spans="1:41" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="282" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C28" s="271">
         <v>0</v>
@@ -15787,7 +15789,7 @@
         <v>0</v>
       </c>
       <c r="E28" s="240" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F28" s="235"/>
       <c r="G28" s="235"/>
@@ -15809,7 +15811,7 @@
     </row>
     <row r="29" spans="1:41" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="283" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C29" s="271">
         <v>0</v>
@@ -15819,7 +15821,7 @@
         <v>0</v>
       </c>
       <c r="E29" s="240" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F29" s="235"/>
       <c r="G29" s="235"/>
@@ -15841,7 +15843,7 @@
     </row>
     <row r="30" spans="1:41" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="284" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C30" s="275">
         <f>C26*C27+C28+C29</f>
@@ -15852,7 +15854,7 @@
         <v>5</v>
       </c>
       <c r="E30" s="277" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F30" s="235"/>
       <c r="G30" s="235"/>
@@ -15874,7 +15876,7 @@
     </row>
     <row r="31" spans="1:41" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="285" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C31" s="286"/>
       <c r="D31" s="287">
@@ -15923,16 +15925,16 @@
       <c r="AO32" s="81"/>
     </row>
     <row r="33" spans="2:41" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="299" t="s">
-        <v>297</v>
-      </c>
-      <c r="C33" s="299"/>
-      <c r="D33" s="299"/>
-      <c r="E33" s="299"/>
-      <c r="F33" s="299"/>
-      <c r="G33" s="299"/>
-      <c r="H33" s="299"/>
-      <c r="I33" s="299"/>
+      <c r="B33" s="314" t="s">
+        <v>296</v>
+      </c>
+      <c r="C33" s="314"/>
+      <c r="D33" s="314"/>
+      <c r="E33" s="314"/>
+      <c r="F33" s="314"/>
+      <c r="G33" s="314"/>
+      <c r="H33" s="314"/>
+      <c r="I33" s="314"/>
       <c r="P33" s="94"/>
       <c r="Q33" s="94"/>
       <c r="R33" s="94"/>
@@ -15949,12 +15951,12 @@
     </row>
     <row r="34" spans="2:41" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C34" s="65"/>
       <c r="D34" s="65"/>
       <c r="E34" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P34" s="94"/>
       <c r="Q34" s="94"/>
@@ -15972,12 +15974,12 @@
     </row>
     <row r="35" spans="2:41" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="68" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C35" s="68"/>
       <c r="D35" s="68"/>
       <c r="E35" s="65" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="P35" s="94"/>
       <c r="Q35" s="94"/>
@@ -15995,14 +15997,14 @@
     </row>
     <row r="36" spans="2:41" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="65" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C36" s="65"/>
-      <c r="D36" s="312"/>
-      <c r="E36" s="312"/>
-      <c r="F36" s="312"/>
-      <c r="G36" s="312"/>
-      <c r="H36" s="312"/>
+      <c r="D36" s="311"/>
+      <c r="E36" s="311"/>
+      <c r="F36" s="311"/>
+      <c r="G36" s="311"/>
+      <c r="H36" s="311"/>
       <c r="P36" s="94"/>
       <c r="Q36" s="94"/>
       <c r="R36" s="94"/>
@@ -16020,19 +16022,19 @@
     </row>
     <row r="37" spans="2:41" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="65" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C37" s="65"/>
       <c r="D37" s="103"/>
       <c r="E37" s="76" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F37" s="104"/>
       <c r="G37" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H37" s="86" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K37" s="98"/>
       <c r="P37" s="94"/>
@@ -16051,19 +16053,19 @@
     </row>
     <row r="38" spans="2:41" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="65" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C38" s="65"/>
       <c r="D38" s="103"/>
       <c r="E38" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="G38" s="76"/>
       <c r="H38" s="86" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K38" s="98"/>
       <c r="P38" s="94"/>
@@ -16082,14 +16084,14 @@
     </row>
     <row r="39" spans="2:41" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="65" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C39" s="65"/>
-      <c r="D39" s="297"/>
-      <c r="E39" s="297"/>
-      <c r="F39" s="297"/>
-      <c r="G39" s="297"/>
-      <c r="H39" s="297"/>
+      <c r="D39" s="303"/>
+      <c r="E39" s="303"/>
+      <c r="F39" s="303"/>
+      <c r="G39" s="303"/>
+      <c r="H39" s="303"/>
       <c r="P39" s="94"/>
       <c r="Q39" s="94"/>
       <c r="R39" s="94"/>
@@ -16107,14 +16109,14 @@
     </row>
     <row r="40" spans="2:41" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="65" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C40" s="65"/>
-      <c r="D40" s="296"/>
-      <c r="E40" s="296"/>
-      <c r="F40" s="296"/>
-      <c r="G40" s="296"/>
-      <c r="H40" s="296"/>
+      <c r="D40" s="312"/>
+      <c r="E40" s="312"/>
+      <c r="F40" s="312"/>
+      <c r="G40" s="312"/>
+      <c r="H40" s="312"/>
       <c r="P40" s="94"/>
       <c r="Q40" s="94"/>
       <c r="R40" s="94"/>
@@ -16132,7 +16134,7 @@
     </row>
     <row r="41" spans="2:41" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="65" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C41" s="65"/>
       <c r="D41" s="68"/>
@@ -16157,14 +16159,14 @@
     </row>
     <row r="42" spans="2:41" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C42" s="65"/>
-      <c r="D42" s="297"/>
-      <c r="E42" s="297"/>
-      <c r="F42" s="297"/>
-      <c r="G42" s="297"/>
-      <c r="H42" s="297"/>
+      <c r="D42" s="303"/>
+      <c r="E42" s="303"/>
+      <c r="F42" s="303"/>
+      <c r="G42" s="303"/>
+      <c r="H42" s="303"/>
       <c r="P42" s="94"/>
       <c r="Q42" s="94"/>
       <c r="R42" s="94"/>
@@ -16182,14 +16184,14 @@
     </row>
     <row r="43" spans="2:41" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="65" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C43" s="65"/>
-      <c r="D43" s="298"/>
-      <c r="E43" s="298"/>
-      <c r="F43" s="298"/>
-      <c r="G43" s="298"/>
-      <c r="H43" s="298"/>
+      <c r="D43" s="313"/>
+      <c r="E43" s="313"/>
+      <c r="F43" s="313"/>
+      <c r="G43" s="313"/>
+      <c r="H43" s="313"/>
       <c r="P43" s="94"/>
       <c r="Q43" s="94"/>
       <c r="R43" s="94"/>
@@ -16207,7 +16209,7 @@
     </row>
     <row r="44" spans="2:41" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="97" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C44" s="65"/>
       <c r="D44" s="219"/>
@@ -16232,14 +16234,14 @@
     </row>
     <row r="45" spans="2:41" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="65" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C45" s="65"/>
-      <c r="D45" s="297"/>
-      <c r="E45" s="297"/>
-      <c r="F45" s="297"/>
-      <c r="G45" s="297"/>
-      <c r="H45" s="297"/>
+      <c r="D45" s="303"/>
+      <c r="E45" s="303"/>
+      <c r="F45" s="303"/>
+      <c r="G45" s="303"/>
+      <c r="H45" s="303"/>
       <c r="P45" s="94"/>
       <c r="Q45" s="94"/>
       <c r="R45" s="94"/>
@@ -16282,7 +16284,7 @@
     </row>
     <row r="47" spans="2:41" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="66" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C47" s="66"/>
       <c r="D47" s="66"/>
@@ -16302,7 +16304,7 @@
     </row>
     <row r="48" spans="2:41" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="67" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C48" s="65"/>
       <c r="D48" s="65"/>
@@ -16322,13 +16324,13 @@
     </row>
     <row r="49" spans="2:42" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="65" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C49" s="65"/>
       <c r="D49" s="65"/>
       <c r="G49" s="105"/>
       <c r="H49" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P49" s="94"/>
       <c r="Q49" s="94"/>
@@ -16346,13 +16348,13 @@
     </row>
     <row r="50" spans="2:42" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="65" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C50" s="65"/>
       <c r="D50" s="65"/>
       <c r="G50" s="106"/>
       <c r="H50" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P50" s="94"/>
       <c r="Q50" s="94"/>
@@ -16385,7 +16387,7 @@
     </row>
     <row r="52" spans="2:42" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="67" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P52" s="94"/>
       <c r="Q52" s="94"/>
@@ -16419,7 +16421,7 @@
     </row>
     <row r="54" spans="2:42" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="65" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C54" s="65"/>
       <c r="D54" s="65"/>
@@ -16439,14 +16441,14 @@
     </row>
     <row r="55" spans="2:42" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="65" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C55" s="65"/>
       <c r="D55" s="65"/>
-      <c r="E55" s="292"/>
-      <c r="F55" s="292"/>
-      <c r="G55" s="292"/>
-      <c r="H55" s="292"/>
+      <c r="E55" s="310"/>
+      <c r="F55" s="310"/>
+      <c r="G55" s="310"/>
+      <c r="H55" s="310"/>
       <c r="P55" s="94"/>
       <c r="Q55" s="94"/>
       <c r="R55" s="94"/>
@@ -16463,7 +16465,7 @@
     </row>
     <row r="56" spans="2:42" s="65" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="65" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D56" s="107"/>
       <c r="E56" s="68"/>
@@ -16494,13 +16496,13 @@
     </row>
     <row r="57" spans="2:42" s="65" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="70" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D57" s="107"/>
-      <c r="E57" s="292"/>
-      <c r="F57" s="292"/>
-      <c r="G57" s="292"/>
-      <c r="H57" s="292"/>
+      <c r="E57" s="310"/>
+      <c r="F57" s="310"/>
+      <c r="G57" s="310"/>
+      <c r="H57" s="310"/>
       <c r="J57" s="98"/>
       <c r="K57" s="98"/>
       <c r="L57" s="98"/>
@@ -16589,7 +16591,7 @@
       </c>
       <c r="E60" s="109"/>
       <c r="G60" s="72" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H60" s="110">
         <f>C29</f>
@@ -16641,7 +16643,7 @@
         <v>36</v>
       </c>
       <c r="D62" s="134" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E62" s="135"/>
       <c r="F62" s="134" t="s">
@@ -16688,7 +16690,7 @@
       <c r="I63" s="141"/>
       <c r="J63" s="178"/>
       <c r="K63" s="65" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
@@ -16721,7 +16723,7 @@
       <c r="I64" s="146"/>
       <c r="J64" s="179"/>
       <c r="K64" s="147" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="N64" s="148"/>
       <c r="O64" s="148"/>
@@ -16756,7 +16758,7 @@
       <c r="I65" s="141"/>
       <c r="J65" s="178"/>
       <c r="K65" s="65" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
@@ -16789,7 +16791,7 @@
       </c>
       <c r="J66" s="178"/>
       <c r="K66" s="65" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
@@ -16824,10 +16826,10 @@
       </c>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
-      <c r="O67" s="292"/>
-      <c r="P67" s="292"/>
-      <c r="Q67" s="292"/>
-      <c r="R67" s="292"/>
+      <c r="O67" s="310"/>
+      <c r="P67" s="310"/>
+      <c r="Q67" s="310"/>
+      <c r="R67" s="310"/>
       <c r="AI67" s="80"/>
       <c r="AJ67" s="89"/>
       <c r="AK67" s="89"/>
@@ -16914,7 +16916,7 @@
         <v>0</v>
       </c>
       <c r="K69" s="82" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L69" s="2"/>
       <c r="M69" s="2"/>
@@ -16930,7 +16932,7 @@
       <c r="B70" s="127"/>
       <c r="C70" s="128"/>
       <c r="D70" s="129" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E70" s="130"/>
       <c r="F70" s="131">
@@ -16954,7 +16956,7 @@
         <v>2</v>
       </c>
       <c r="K70" s="177" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L70" s="2"/>
       <c r="M70" s="2"/>
@@ -16970,7 +16972,7 @@
       <c r="B71" s="65"/>
       <c r="C71" s="85"/>
       <c r="D71" s="129" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E71" s="130"/>
       <c r="F71" s="197">
@@ -17006,7 +17008,7 @@
       <c r="B72" s="65"/>
       <c r="C72" s="85"/>
       <c r="D72" s="200" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E72" s="201"/>
       <c r="F72" s="202"/>
@@ -17036,7 +17038,7 @@
       <c r="B73" s="65"/>
       <c r="C73" s="85"/>
       <c r="D73" s="176" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E73" s="115"/>
       <c r="G73" s="153"/>
@@ -17065,7 +17067,7 @@
       <c r="B74" s="65"/>
       <c r="C74" s="85"/>
       <c r="D74" s="176" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E74" s="115"/>
       <c r="G74" s="153"/>
@@ -17094,7 +17096,7 @@
       <c r="B75" s="65"/>
       <c r="C75" s="85"/>
       <c r="D75" s="206" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E75" s="207"/>
       <c r="F75" s="104"/>
@@ -17156,13 +17158,13 @@
     </row>
     <row r="77" spans="1:42" s="85" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="68" t="s">
-        <v>285</v>
-      </c>
-      <c r="C77" s="297"/>
-      <c r="D77" s="297"/>
-      <c r="E77" s="297"/>
-      <c r="F77" s="297"/>
-      <c r="G77" s="297"/>
+        <v>284</v>
+      </c>
+      <c r="C77" s="303"/>
+      <c r="D77" s="303"/>
+      <c r="E77" s="303"/>
+      <c r="F77" s="303"/>
+      <c r="G77" s="303"/>
       <c r="K77" s="101"/>
       <c r="L77" s="101"/>
       <c r="M77" s="192"/>
@@ -17220,7 +17222,7 @@
       <c r="L78" s="98"/>
       <c r="M78" s="184"/>
       <c r="N78" s="107" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O78" s="222">
         <f>Rates!E31</f>
@@ -17264,16 +17266,16 @@
     </row>
     <row r="79" spans="1:42" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="67" t="s">
+        <v>75</v>
+      </c>
+      <c r="C79" s="232" t="s">
         <v>76</v>
-      </c>
-      <c r="C79" s="232" t="s">
-        <v>77</v>
       </c>
       <c r="D79" s="65"/>
       <c r="K79" s="98"/>
       <c r="M79" s="174"/>
       <c r="N79" s="223" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O79" s="224">
         <f>Rates!E40</f>
@@ -17309,19 +17311,19 @@
     </row>
     <row r="80" spans="1:42" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B80" s="65" t="s">
+        <v>78</v>
+      </c>
+      <c r="C80" s="72" t="s">
         <v>79</v>
       </c>
-      <c r="C80" s="72" t="s">
+      <c r="D80" s="315"/>
+      <c r="E80" s="315"/>
+      <c r="F80" s="72" t="s">
         <v>80</v>
-      </c>
-      <c r="D80" s="293"/>
-      <c r="E80" s="293"/>
-      <c r="F80" s="72" t="s">
-        <v>81</v>
       </c>
       <c r="G80" s="103"/>
       <c r="M80" s="120" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N80" s="225"/>
       <c r="O80" s="91"/>
@@ -17346,10 +17348,10 @@
     </row>
     <row r="81" spans="2:41" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="65" t="s">
+        <v>81</v>
+      </c>
+      <c r="C81" s="72" t="s">
         <v>82</v>
-      </c>
-      <c r="C81" s="72" t="s">
-        <v>83</v>
       </c>
       <c r="D81" s="119"/>
       <c r="M81" s="175" t="s">
@@ -17397,12 +17399,12 @@
     <row r="82" spans="2:41" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="65"/>
       <c r="C82" s="72" t="s">
+        <v>79</v>
+      </c>
+      <c r="D82" s="316"/>
+      <c r="E82" s="316"/>
+      <c r="F82" s="72" t="s">
         <v>80</v>
-      </c>
-      <c r="D82" s="294"/>
-      <c r="E82" s="294"/>
-      <c r="F82" s="72" t="s">
-        <v>81</v>
       </c>
       <c r="G82" s="103"/>
       <c r="M82" s="123" t="s">
@@ -17449,14 +17451,14 @@
     </row>
     <row r="83" spans="2:41" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="65" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C83" s="65"/>
-      <c r="D83" s="295"/>
-      <c r="E83" s="295"/>
-      <c r="F83" s="295"/>
-      <c r="G83" s="295"/>
-      <c r="H83" s="295"/>
+      <c r="D83" s="317"/>
+      <c r="E83" s="317"/>
+      <c r="F83" s="317"/>
+      <c r="G83" s="317"/>
+      <c r="H83" s="317"/>
       <c r="M83" s="175" t="s">
         <v>25</v>
       </c>
@@ -17601,7 +17603,7 @@
       <c r="C86" s="65"/>
       <c r="D86" s="98"/>
       <c r="M86" s="176" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N86" s="2"/>
       <c r="O86" s="2"/>
@@ -17623,7 +17625,7 @@
     <row r="87" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B87" s="65"/>
       <c r="M87" s="206" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N87" s="104"/>
       <c r="O87" s="104"/>
@@ -17648,7 +17650,7 @@
     </row>
     <row r="88" spans="2:41" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="67" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="N88" s="228"/>
       <c r="O88" s="228"/>
@@ -17663,11 +17665,11 @@
     <row r="89" spans="2:41" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="65"/>
       <c r="C89" s="65"/>
-      <c r="D89" s="296"/>
-      <c r="E89" s="296"/>
-      <c r="F89" s="296"/>
-      <c r="G89" s="296"/>
-      <c r="H89" s="296"/>
+      <c r="D89" s="312"/>
+      <c r="E89" s="312"/>
+      <c r="F89" s="312"/>
+      <c r="G89" s="312"/>
+      <c r="H89" s="312"/>
       <c r="N89" s="228"/>
       <c r="O89" s="228"/>
       <c r="AB89" s="116"/>
@@ -17686,13 +17688,13 @@
     </row>
     <row r="90" spans="2:41" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="236" t="s">
+        <v>286</v>
+      </c>
+      <c r="C90" s="110" t="s">
         <v>287</v>
       </c>
-      <c r="C90" s="110" t="s">
+      <c r="D90" s="236" t="s">
         <v>288</v>
-      </c>
-      <c r="D90" s="236" t="s">
-        <v>289</v>
       </c>
       <c r="E90" s="65"/>
       <c r="F90" s="65"/>
@@ -18077,11 +18079,16 @@
     <protectedRange sqref="D30" name="Range1"/>
   </protectedRanges>
   <mergeCells count="31">
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="O67:R67"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D83:H83"/>
+    <mergeCell ref="D89:H89"/>
+    <mergeCell ref="D42:H42"/>
+    <mergeCell ref="D43:H43"/>
+    <mergeCell ref="D45:H45"/>
+    <mergeCell ref="E55:H55"/>
+    <mergeCell ref="B33:I33"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="C23:I23"/>
     <mergeCell ref="B24:B25"/>
@@ -18098,16 +18105,11 @@
     <mergeCell ref="D39:H39"/>
     <mergeCell ref="D36:H36"/>
     <mergeCell ref="D40:H40"/>
-    <mergeCell ref="D42:H42"/>
-    <mergeCell ref="D43:H43"/>
-    <mergeCell ref="D45:H45"/>
-    <mergeCell ref="E55:H55"/>
-    <mergeCell ref="B33:I33"/>
-    <mergeCell ref="O67:R67"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D83:H83"/>
-    <mergeCell ref="D89:H89"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
   </mergeCells>
   <conditionalFormatting sqref="C28:C29">
     <cfRule type="cellIs" dxfId="21" priority="2" operator="greaterThan">
@@ -18783,10 +18785,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="94" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1" s="94" t="s">
         <v>227</v>
-      </c>
-      <c r="B1" s="94" t="s">
-        <v>228</v>
       </c>
       <c r="C1" s="94"/>
       <c r="D1" s="94"/>
@@ -18794,13 +18796,13 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="94" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B2" s="94"/>
       <c r="C2" s="94"/>
       <c r="E2" s="94"/>
       <c r="K2" s="94" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -18831,13 +18833,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="94" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G1" s="91" t="s">
+        <v>237</v>
+      </c>
+      <c r="H1" s="91" t="s">
         <v>238</v>
-      </c>
-      <c r="H1" s="91" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -18845,22 +18847,22 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="156" t="s">
+        <v>231</v>
+      </c>
+      <c r="B3" s="156" t="s">
         <v>232</v>
       </c>
-      <c r="B3" s="156" t="s">
+      <c r="C3" s="156" t="s">
         <v>233</v>
       </c>
-      <c r="C3" s="156" t="s">
+      <c r="D3" s="156" t="s">
         <v>234</v>
       </c>
-      <c r="D3" s="156" t="s">
+      <c r="E3" s="156" t="s">
         <v>235</v>
       </c>
-      <c r="E3" s="156" t="s">
+      <c r="F3" s="156" t="s">
         <v>236</v>
-      </c>
-      <c r="F3" s="156" t="s">
-        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -18884,15 +18886,15 @@
   <sheetData>
     <row r="3" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B3" s="156" t="s">
+        <v>241</v>
+      </c>
+      <c r="AA3" s="156" t="s">
         <v>242</v>
-      </c>
-      <c r="AA3" s="156" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="49" spans="34:34" x14ac:dyDescent="0.25">
       <c r="AH49" s="156" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -18925,10 +18927,10 @@
   <sheetData>
     <row r="1" spans="2:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>0</v>
@@ -18936,10 +18938,10 @@
     </row>
     <row r="2" spans="2:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K2" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>277</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="3" spans="2:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18952,7 +18954,7 @@
       <c r="H3" s="90"/>
       <c r="I3" s="90"/>
       <c r="K3" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>3</v>
@@ -18968,7 +18970,7 @@
       <c r="H4" s="90"/>
       <c r="I4" s="90"/>
       <c r="K4" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>3</v>
@@ -19097,13 +19099,13 @@
       <c r="C14" s="20"/>
       <c r="D14" s="21"/>
       <c r="E14" s="237" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F14" s="237" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G14" s="237" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H14" s="237" t="s">
         <v>6</v>
@@ -19503,13 +19505,13 @@
       <c r="C30" s="256"/>
       <c r="D30" s="257"/>
       <c r="E30" s="237" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F30" s="237" t="s">
+        <v>289</v>
+      </c>
+      <c r="G30" s="237" t="s">
         <v>290</v>
-      </c>
-      <c r="G30" s="237" t="s">
-        <v>291</v>
       </c>
       <c r="H30" s="237" t="s">
         <v>6</v>
@@ -19588,7 +19590,7 @@
     <row r="33" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="24"/>
       <c r="C33" s="258" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D33" s="259">
         <v>1</v>
@@ -19598,7 +19600,7 @@
         <v>5</v>
       </c>
       <c r="F33" s="323" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G33" s="260"/>
       <c r="H33" s="260"/>
@@ -19651,7 +19653,7 @@
         <v>0</v>
       </c>
       <c r="F35" s="264" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G35" s="30"/>
       <c r="H35" s="30"/>
@@ -19670,7 +19672,7 @@
     <row r="36" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="24"/>
       <c r="C36" s="236" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D36" s="262">
         <v>0</v>
@@ -19680,7 +19682,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="264" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G36" s="30"/>
       <c r="H36" s="30"/>
@@ -19699,7 +19701,7 @@
     <row r="37" spans="2:22" s="47" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="62"/>
       <c r="C37" s="265" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D37" s="266">
         <f>D33*D34+D35+D36</f>
@@ -19710,7 +19712,7 @@
         <v>5</v>
       </c>
       <c r="F37" s="268" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G37" s="30"/>
       <c r="H37" s="30"/>
@@ -19905,52 +19907,52 @@
   <sheetData>
     <row r="1" spans="1:12" s="65" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="152" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="153" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="68" t="s">
         <v>88</v>
-      </c>
-      <c r="B2" s="68" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="153"/>
       <c r="B3" s="68" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="154" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="154" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="299" t="s">
-        <v>92</v>
-      </c>
-      <c r="C8" s="299"/>
-      <c r="D8" s="299"/>
-      <c r="E8" s="299"/>
-      <c r="F8" s="299"/>
-      <c r="G8" s="299"/>
-      <c r="H8" s="299"/>
-      <c r="I8" s="299"/>
-      <c r="J8" s="299"/>
-      <c r="K8" s="299"/>
-      <c r="L8" s="299"/>
+      <c r="B8" s="314" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="314"/>
+      <c r="D8" s="314"/>
+      <c r="E8" s="314"/>
+      <c r="F8" s="314"/>
+      <c r="G8" s="314"/>
+      <c r="H8" s="314"/>
+      <c r="I8" s="314"/>
+      <c r="J8" s="314"/>
+      <c r="K8" s="314"/>
+      <c r="L8" s="314"/>
     </row>
     <row r="9" spans="1:12" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="325" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C9" s="325"/>
       <c r="D9" s="325"/>
@@ -19965,7 +19967,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" s="326" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" s="326"/>
       <c r="D10" s="326"/>
@@ -19989,15 +19991,15 @@
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="156" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="327" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C14" s="327"/>
       <c r="D14" s="327"/>
@@ -20012,7 +20014,7 @@
     </row>
     <row r="15" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="325" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C15" s="325"/>
       <c r="D15" s="325"/>
@@ -20027,7 +20029,7 @@
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="325" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C16" s="325"/>
       <c r="D16" s="325"/>
@@ -20042,17 +20044,17 @@
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="157" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B18" s="157" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:12" s="65" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="325" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C19" s="325"/>
       <c r="D19" s="325"/>
@@ -20067,10 +20069,10 @@
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>102</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>103</v>
       </c>
       <c r="D20" s="158"/>
       <c r="E20" s="158"/>
@@ -20087,30 +20089,30 @@
     </row>
     <row r="23" spans="1:12" s="108" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="108" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" s="108" t="s">
         <v>104</v>
-      </c>
-      <c r="B23" s="108" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:12" s="108" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:12" s="108" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:12" s="108" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:12" s="108" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:12" s="108" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -20118,136 +20120,136 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="159" t="s">
         <v>110</v>
       </c>
-      <c r="B29" s="159" t="s">
+      <c r="D29" s="157" t="s">
         <v>111</v>
-      </c>
-      <c r="D29" s="157" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B30" s="159" t="s">
         <v>113</v>
       </c>
-      <c r="B30" s="159" t="s">
+      <c r="D30" s="157" t="s">
         <v>114</v>
-      </c>
-      <c r="D30" s="157" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" s="159" t="s">
         <v>116</v>
-      </c>
-      <c r="B31" s="159" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="160" t="s">
+        <v>119</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D35" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D40" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D41" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D42" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D43" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D44" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D45" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D46" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D47" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D48" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -20292,43 +20294,43 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="161" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:8" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="162" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" s="163" t="s">
         <v>142</v>
       </c>
-      <c r="B5" s="163" t="s">
+      <c r="C5" s="164" t="s">
         <v>143</v>
       </c>
-      <c r="C5" s="164" t="s">
+      <c r="D5" s="164" t="s">
         <v>144</v>
       </c>
-      <c r="D5" s="164" t="s">
+      <c r="E5" s="163" t="s">
         <v>145</v>
       </c>
-      <c r="E5" s="163" t="s">
+      <c r="F5" s="163" t="s">
         <v>146</v>
       </c>
-      <c r="F5" s="163" t="s">
+      <c r="G5" s="328" t="s">
         <v>147</v>
-      </c>
-      <c r="G5" s="328" t="s">
-        <v>148</v>
       </c>
       <c r="H5" s="328"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="99" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B8" s="165">
         <v>163</v>
@@ -20340,18 +20342,18 @@
         <v>0.8</v>
       </c>
       <c r="E8" s="165" t="s">
+        <v>149</v>
+      </c>
+      <c r="F8" s="165" t="s">
+        <v>149</v>
+      </c>
+      <c r="G8" s="99" t="s">
         <v>150</v>
-      </c>
-      <c r="F8" s="165" t="s">
-        <v>150</v>
-      </c>
-      <c r="G8" s="99" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="99" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B9" s="165"/>
       <c r="C9" s="166"/>
@@ -20361,12 +20363,12 @@
         <v>0.03</v>
       </c>
       <c r="G9" s="99" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B10" s="91">
         <v>615</v>
@@ -20384,35 +20386,35 @@
         <v>0.1</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B11" s="91">
         <v>284</v>
       </c>
       <c r="C11" s="167" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D11" s="167" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E11" s="91" t="s">
+        <v>156</v>
+      </c>
+      <c r="F11" s="91" t="s">
         <v>157</v>
       </c>
-      <c r="F11" s="91" t="s">
+      <c r="G11" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B12" s="91">
         <v>154</v>
@@ -20424,18 +20426,18 @@
         <v>7.7</v>
       </c>
       <c r="E12" s="91" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F12" s="91" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B13" s="91">
         <v>92</v>
@@ -20447,18 +20449,18 @@
         <v>1.2</v>
       </c>
       <c r="E13" s="91" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F13" s="91" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="99" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B14" s="165">
         <v>96</v>
@@ -20470,18 +20472,18 @@
         <v>2.4</v>
       </c>
       <c r="E14" s="165" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F14" s="165" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G14" s="99" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="99" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B15" s="165">
         <v>238</v>
@@ -20493,18 +20495,18 @@
         <v>2.4</v>
       </c>
       <c r="E15" s="165" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F15" s="165" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G15" s="99" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="99" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B16" s="165"/>
       <c r="C16" s="166"/>
@@ -20519,7 +20521,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B17" s="91">
         <v>229</v>
@@ -20531,27 +20533,27 @@
         <v>1</v>
       </c>
       <c r="E17" s="91" t="s">
+        <v>168</v>
+      </c>
+      <c r="F17" s="91" t="s">
+        <v>157</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="F17" s="91" t="s">
-        <v>158</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B18" s="91">
         <v>264</v>
       </c>
       <c r="C18" s="167" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D18" s="167" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E18" s="91">
         <v>3.8</v>
@@ -20560,12 +20562,12 @@
         <v>0.1</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B19" s="91">
         <v>58</v>
@@ -20577,18 +20579,18 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="E19" s="91" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F19" s="91" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B20" s="91">
         <v>120</v>
@@ -20606,21 +20608,21 @@
         <v>0.12</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B21" s="91">
         <v>348</v>
       </c>
       <c r="C21" s="167" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D21" s="167" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E21" s="91">
         <v>2.9</v>
@@ -20629,21 +20631,21 @@
         <v>0.1</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B22" s="91">
         <v>511</v>
       </c>
       <c r="C22" s="167" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D22" s="167" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E22" s="91">
         <v>2</v>
@@ -20652,21 +20654,21 @@
         <v>0.1</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B23" s="91">
         <v>524</v>
       </c>
       <c r="C23" s="167" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D23" s="167" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E23" s="91">
         <v>1.9</v>
@@ -20675,12 +20677,12 @@
         <v>0.1</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B24" s="91">
         <v>79</v>
@@ -20692,18 +20694,18 @@
         <v>0.4</v>
       </c>
       <c r="E24" s="91" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F24" s="91" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B25" s="91">
         <v>292</v>
@@ -20721,21 +20723,21 @@
         <v>0.1</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B26" s="91">
         <v>468</v>
       </c>
       <c r="C26" s="167" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D26" s="167" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E26" s="91">
         <v>2.1</v>
@@ -20744,12 +20746,12 @@
         <v>0.1</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B27" s="91">
         <v>603</v>
@@ -20761,24 +20763,24 @@
         <v>0.1</v>
       </c>
       <c r="E27" s="91" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F27" s="91" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B28" s="91">
         <v>308</v>
       </c>
       <c r="C28" s="167" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D28" s="167" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E28" s="91">
         <v>3.2</v>
@@ -20787,21 +20789,21 @@
         <v>0.1</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B29" s="91">
         <v>1000</v>
       </c>
       <c r="C29" s="167" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D29" s="167" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E29" s="91">
         <v>0.5</v>
@@ -20810,12 +20812,12 @@
         <v>0.05</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B30" s="91">
         <v>2000</v>
@@ -20827,18 +20829,18 @@
         <v>0.1</v>
       </c>
       <c r="E30" s="91" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F30" s="91" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B31" s="91">
         <v>288</v>
@@ -20856,12 +20858,12 @@
         <v>0.01</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B32" s="91">
         <v>82</v>
@@ -20873,18 +20875,18 @@
         <v>0.41</v>
       </c>
       <c r="E32" s="91" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F32" s="91" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B33" s="91">
         <v>65</v>
@@ -20902,21 +20904,21 @@
         <v>0.02</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B34" s="91">
         <v>431</v>
       </c>
       <c r="C34" s="167" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D34" s="167" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E34" s="91">
         <v>2.2999999999999998</v>
@@ -20925,44 +20927,44 @@
         <v>0.1</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B35" s="91">
         <v>538</v>
       </c>
       <c r="C35" s="167" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D35" s="167" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E35" s="91" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F35" s="91" t="s">
+        <v>157</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B36" s="91">
         <v>114</v>
       </c>
       <c r="C36" s="167" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D36" s="167" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E36" s="91">
         <v>4.4000000000000004</v>
@@ -20971,35 +20973,35 @@
         <v>0.05</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B37" s="91">
         <v>583</v>
       </c>
       <c r="C37" s="167" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D37" s="167" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E37" s="91" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F37" s="91" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="99" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B38" s="165">
         <v>121</v>
@@ -21011,18 +21013,18 @@
         <v>1</v>
       </c>
       <c r="E38" s="165" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F38" s="165" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G38" s="99" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B39" s="91">
         <v>628</v>
@@ -21034,41 +21036,41 @@
         <v>0.1</v>
       </c>
       <c r="E39" s="91" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F39" s="91">
         <v>0.05</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B40" s="91">
         <v>1228</v>
       </c>
       <c r="C40" s="167" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D40" s="167">
         <v>0.6</v>
       </c>
       <c r="E40" s="91" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F40" s="91">
         <v>0.05</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="99" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B41" s="165">
         <v>60</v>
@@ -21080,18 +21082,18 @@
         <v>3</v>
       </c>
       <c r="E41" s="165" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F41" s="165" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G41" s="99" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B42" s="91">
         <v>392</v>
@@ -21103,13 +21105,13 @@
         <v>0.1</v>
       </c>
       <c r="E42" s="91" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F42" s="91" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -21122,119 +21124,119 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="99" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C45" s="168"/>
       <c r="D45" s="168"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="99" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C46" s="168"/>
       <c r="D46" s="168"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="99" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C47" s="168"/>
       <c r="D47" s="168"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="99" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C48" s="168"/>
       <c r="D48" s="168"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="99" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C49" s="168"/>
       <c r="D49" s="168"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="99" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C50" s="168"/>
       <c r="D50" s="168"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="99" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C51" s="168"/>
       <c r="D51" s="168"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="99" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C52" s="168"/>
       <c r="D52" s="168"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="99" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C53" s="168"/>
       <c r="D53" s="168"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="99" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C54" s="168"/>
       <c r="D54" s="168"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="169" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C55" s="168"/>
       <c r="D55" s="168"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="169" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C56" s="168"/>
       <c r="D56" s="168"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="99" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C57" s="168"/>
       <c r="D57" s="168"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="169" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C58" s="168"/>
       <c r="D58" s="168"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="169" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C59" s="168"/>
       <c r="D59" s="168"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="169" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C60" s="168"/>
       <c r="D60" s="168"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="99" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C61" s="168"/>
       <c r="D61" s="168"/>

</xml_diff>